<commit_message>
just created the django project and it is up and running
</commit_message>
<xml_diff>
--- a/PopularPackages/PyExcel/transactions2.xlsx
+++ b/PopularPackages/PyExcel/transactions2.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="500" visibility="visible" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1" refMode="A1" iterate="0" iterateCount="100" iterateDelta="0.001"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1" iterate="0" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[$$-C09]#,##0.00;[RED]\-[$$-C09]#,##0.00"/>
+    <numFmt formatCode="[$$-C09]#,##0.00;[RED]\-[$$-C09]#,##0.00" numFmtId="164"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -59,37 +59,37 @@
     </border>
   </borders>
   <cellStyleXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="2" builtinId="6"/>
-    <cellStyle name="Currency" xfId="3" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Percent" xfId="5" builtinId="5"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="3" name="Comma" xfId="1"/>
+    <cellStyle builtinId="6" name="Comma [0]" xfId="2"/>
+    <cellStyle builtinId="4" name="Currency" xfId="3"/>
+    <cellStyle builtinId="7" name="Currency [0]" xfId="4"/>
+    <cellStyle builtinId="5" name="Percent" xfId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -385,16 +385,16 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" workbookViewId="0" zoomScale="250" zoomScaleNormal="250" zoomScalePageLayoutView="100">
+      <selection activeCell="C5" activeCellId="0" pane="topLeft" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" zeroHeight="0" outlineLevelRow="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="12.8" outlineLevelRow="0" zeroHeight="0"/>
   <cols>
-    <col width="11.52" customWidth="1" style="2" min="1" max="1025"/>
+    <col customWidth="1" max="1025" min="1" style="2" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" ht="12.8" customHeight="1" s="3">
+    <row customHeight="1" ht="12.8" r="1" s="3">
       <c r="A1" s="2" t="inlineStr">
         <is>
           <t>transaction_id</t>
@@ -411,7 +411,7 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="12.8" customHeight="1" s="3">
+    <row customHeight="1" ht="12.8" r="2" s="3">
       <c r="A2" s="2" t="n">
         <v>1001</v>
       </c>
@@ -422,7 +422,7 @@
         <v>5.95</v>
       </c>
     </row>
-    <row r="3" ht="12.8" customHeight="1" s="3">
+    <row customHeight="1" ht="12.8" r="3" s="3">
       <c r="A3" s="2" t="n">
         <v>1002</v>
       </c>
@@ -433,7 +433,7 @@
         <v>6.95</v>
       </c>
     </row>
-    <row r="4" ht="12.8" customHeight="1" s="3">
+    <row customHeight="1" ht="12.8" r="4" s="3">
       <c r="A4" s="2" t="n">
         <v>1003</v>
       </c>
@@ -456,10 +456,10 @@
       </c>
     </row>
   </sheetData>
-  <printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0" gridLinesSet="1"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup orientation="portrait" paperSize="9" scale="100" fitToHeight="1" fitToWidth="1" firstPageNumber="1" useFirstPageNumber="1" pageOrder="downThenOver" blackAndWhite="0" draft="0" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentOddEven="0" differentFirst="0">
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
+  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageSetup blackAndWhite="0" copies="1" draft="0" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="1" verticalDpi="300"/>
+  <headerFooter differentFirst="0" differentOddEven="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12 &amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12 Page &amp;P</oddFooter>
     <evenHeader/>

</xml_diff>